<commit_message>
Excel, Python and R files added
</commit_message>
<xml_diff>
--- a/DA using R/W2/Correlation&Regression.xlsx
+++ b/DA using R/W2/Correlation&Regression.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23801"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23901"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\AjitC\Desktop\Data Analyst Course\StatisticsWithR\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\AjitC\Desktop\Data Analyst Course\Data-Analyst-Course\DA using R\W2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0CFEC923-D00F-46EF-A7FB-6D4EC51BD4E1}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CE447C6E-B747-4635-A58E-BD7F18BDFEA1}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="2" xr2:uid="{E1359F83-D15D-42CE-82D8-052BCC73DE87}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{E1359F83-D15D-42CE-82D8-052BCC73DE87}"/>
   </bookViews>
   <sheets>
     <sheet name="W3" sheetId="8" r:id="rId1"/>
@@ -291,6 +291,22 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -300,22 +316,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2068,10 +2068,10 @@
   </cols>
   <sheetData>
     <row r="4" spans="10:11" x14ac:dyDescent="0.3">
-      <c r="J4" s="8" t="s">
+      <c r="J4" s="5" t="s">
         <v>36</v>
       </c>
-      <c r="K4" s="9" t="s">
+      <c r="K4" s="6" t="s">
         <v>37</v>
       </c>
     </row>
@@ -2135,7 +2135,7 @@
       <c r="J12" s="4" t="s">
         <v>42</v>
       </c>
-      <c r="K12" s="10" t="s">
+      <c r="K12" s="7" t="s">
         <v>41</v>
       </c>
     </row>
@@ -2165,8 +2165,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A53511EF-58C4-44BF-8073-E7CECCFB8D3D}">
   <dimension ref="A2:I15"/>
   <sheetViews>
-    <sheetView zoomScale="98" workbookViewId="0">
-      <selection activeCell="H16" sqref="H16"/>
+    <sheetView tabSelected="1" zoomScale="98" workbookViewId="0">
+      <selection activeCell="O5" sqref="O5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2189,7 +2189,7 @@
       <c r="F2" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="I2" s="11"/>
+      <c r="I2" s="8"/>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B3" s="4" t="s">
@@ -2208,7 +2208,7 @@
         <f>SUM(C3:E3)</f>
         <v>2</v>
       </c>
-      <c r="I3" s="11"/>
+      <c r="I3" s="8"/>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B4" s="4" t="s">
@@ -2227,7 +2227,7 @@
         <f>SUM(C4:E4)</f>
         <v>2</v>
       </c>
-      <c r="I4" s="11"/>
+      <c r="I4" s="8"/>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B5" s="4" t="s">
@@ -2246,7 +2246,7 @@
         <f t="shared" ref="F5:F6" si="0">SUM(C5:E5)</f>
         <v>3</v>
       </c>
-      <c r="I5" s="11"/>
+      <c r="I5" s="8"/>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B6" s="4" t="s">
@@ -2265,7 +2265,7 @@
         <f t="shared" si="0"/>
         <v>3</v>
       </c>
-      <c r="I6" s="11"/>
+      <c r="I6" s="8"/>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B7" s="4" t="s">
@@ -2287,16 +2287,16 @@
         <f>SUM(F3:F6)</f>
         <v>10</v>
       </c>
-      <c r="I7" s="12"/>
+      <c r="I7" s="9"/>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="B9" s="13" t="s">
+      <c r="B9" s="12" t="s">
         <v>43</v>
       </c>
-      <c r="C9" s="13"/>
-      <c r="D9" s="13"/>
-      <c r="E9" s="13"/>
-      <c r="F9" s="13"/>
+      <c r="C9" s="12"/>
+      <c r="D9" s="12"/>
+      <c r="E9" s="12"/>
+      <c r="F9" s="12"/>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B10" s="4"/>
@@ -2314,92 +2314,92 @@
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A11" s="14" t="s">
+      <c r="A11" s="11" t="s">
         <v>36</v>
       </c>
       <c r="B11" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="C11" s="15">
-        <f>C3/$C$7</f>
-        <v>0.66666666666666663</v>
-      </c>
-      <c r="D11" s="15">
-        <f>D3/$D$7</f>
+      <c r="C11" s="10">
+        <f>C3/F7</f>
+        <v>0.2</v>
+      </c>
+      <c r="D11" s="10">
+        <f>D3/F7</f>
         <v>0</v>
       </c>
-      <c r="E11" s="15">
-        <f>E3/$E$7</f>
+      <c r="E11" s="10">
+        <f>E3/F7</f>
         <v>0</v>
       </c>
-      <c r="F11" s="15">
+      <c r="F11" s="10">
         <f>F3/$F$7</f>
         <v>0.2</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A12" s="14"/>
+      <c r="A12" s="11"/>
       <c r="B12" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="C12" s="15">
-        <f t="shared" ref="C12:C15" si="2">C4/$C$7</f>
-        <v>0.33333333333333331</v>
-      </c>
-      <c r="D12" s="15">
-        <f t="shared" ref="D12:D15" si="3">D4/$D$7</f>
+      <c r="C12" s="10">
+        <f>C4/F7</f>
+        <v>0.1</v>
+      </c>
+      <c r="D12" s="10">
+        <f>D4/F7</f>
         <v>0</v>
       </c>
-      <c r="E12" s="15">
-        <f t="shared" ref="E12:E15" si="4">E4/$E$7</f>
-        <v>0.25</v>
-      </c>
-      <c r="F12" s="15">
-        <f t="shared" ref="F12:F15" si="5">F4/$F$7</f>
+      <c r="E12" s="10">
+        <f>E4/F7</f>
+        <v>0.1</v>
+      </c>
+      <c r="F12" s="10">
+        <f>F4/$F$7</f>
         <v>0.2</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A13" s="14"/>
+      <c r="A13" s="11"/>
       <c r="B13" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="C13" s="15">
-        <f t="shared" si="2"/>
+      <c r="C13" s="10">
+        <f>C5/F7</f>
         <v>0</v>
       </c>
-      <c r="D13" s="15">
-        <f t="shared" si="3"/>
+      <c r="D13" s="10">
+        <f>D5/F7</f>
         <v>0</v>
       </c>
-      <c r="E13" s="15">
-        <f t="shared" si="4"/>
-        <v>0.75</v>
-      </c>
-      <c r="F13" s="15">
-        <f t="shared" si="5"/>
+      <c r="E13" s="10">
+        <f>E5/F7</f>
         <v>0.3</v>
       </c>
+      <c r="F13" s="10">
+        <f t="shared" ref="F12:F15" si="2">F5/$F$7</f>
+        <v>0.3</v>
+      </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A14" s="14"/>
+      <c r="A14" s="11"/>
       <c r="B14" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="C14" s="15">
-        <f t="shared" si="2"/>
+      <c r="C14" s="10">
+        <f>C6/F7</f>
         <v>0</v>
       </c>
-      <c r="D14" s="15">
-        <f t="shared" si="3"/>
-        <v>1</v>
-      </c>
-      <c r="E14" s="15">
-        <f t="shared" si="4"/>
+      <c r="D14" s="10">
+        <f>D6/F7</f>
+        <v>0.3</v>
+      </c>
+      <c r="E14" s="10">
+        <f>E6/F7</f>
         <v>0</v>
       </c>
-      <c r="F14" s="15">
-        <f t="shared" si="5"/>
+      <c r="F14" s="10">
+        <f>F6/$F$7</f>
         <v>0.3</v>
       </c>
     </row>
@@ -2407,20 +2407,20 @@
       <c r="B15" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="C15" s="15">
-        <f t="shared" si="2"/>
-        <v>1</v>
-      </c>
-      <c r="D15" s="15">
-        <f t="shared" si="3"/>
-        <v>1</v>
-      </c>
-      <c r="E15" s="15">
-        <f t="shared" si="4"/>
-        <v>1</v>
-      </c>
-      <c r="F15" s="15">
-        <f t="shared" si="5"/>
+      <c r="C15" s="10">
+        <f>C7/F7</f>
+        <v>0.3</v>
+      </c>
+      <c r="D15" s="10">
+        <f>D7/F7</f>
+        <v>0.3</v>
+      </c>
+      <c r="E15" s="10">
+        <f>E7/F7</f>
+        <v>0.4</v>
+      </c>
+      <c r="F15" s="10">
+        <f>F7/$F$7</f>
         <v>1</v>
       </c>
     </row>
@@ -2437,8 +2437,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8D6F5278-6E2C-4BB1-9E4C-8261453B12AB}">
   <dimension ref="A1:F23"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D18" sqref="D18"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2601,10 +2601,10 @@
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="C16" s="8" t="s">
+      <c r="C16" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="D16" s="8" t="s">
+      <c r="D16" s="5" t="s">
         <v>17</v>
       </c>
       <c r="F16">
@@ -2613,10 +2613,10 @@
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="C17" s="8" t="s">
+      <c r="C17" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="D17" s="8" t="s">
+      <c r="D17" s="5" t="s">
         <v>20</v>
       </c>
       <c r="F17">
@@ -2652,10 +2652,10 @@
       <c r="B21" s="1"/>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="C23" s="5" t="s">
+      <c r="C23" s="13" t="s">
         <v>25</v>
       </c>
-      <c r="D23" s="6"/>
+      <c r="D23" s="14"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -2694,12 +2694,12 @@
       <c r="C2">
         <v>47</v>
       </c>
-      <c r="F2" s="7" t="s">
+      <c r="F2" s="15" t="s">
         <v>32</v>
       </c>
-      <c r="G2" s="6"/>
-      <c r="H2" s="6"/>
-      <c r="I2" s="6"/>
+      <c r="G2" s="14"/>
+      <c r="H2" s="14"/>
+      <c r="I2" s="14"/>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
@@ -2711,10 +2711,10 @@
       <c r="C3">
         <v>49.9</v>
       </c>
-      <c r="F3" s="6"/>
-      <c r="G3" s="6"/>
-      <c r="H3" s="6"/>
-      <c r="I3" s="6"/>
+      <c r="F3" s="14"/>
+      <c r="G3" s="14"/>
+      <c r="H3" s="14"/>
+      <c r="I3" s="14"/>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
@@ -2726,10 +2726,10 @@
       <c r="C4">
         <v>55.1</v>
       </c>
-      <c r="F4" s="6"/>
-      <c r="G4" s="6"/>
-      <c r="H4" s="6"/>
-      <c r="I4" s="6"/>
+      <c r="F4" s="14"/>
+      <c r="G4" s="14"/>
+      <c r="H4" s="14"/>
+      <c r="I4" s="14"/>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
@@ -2741,10 +2741,10 @@
       <c r="C5">
         <v>60.9</v>
       </c>
-      <c r="F5" s="6"/>
-      <c r="G5" s="6"/>
-      <c r="H5" s="6"/>
-      <c r="I5" s="6"/>
+      <c r="F5" s="14"/>
+      <c r="G5" s="14"/>
+      <c r="H5" s="14"/>
+      <c r="I5" s="14"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -2758,78 +2758,78 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DDF5BBAD-1333-4B2D-A7FE-9B3A823D4BDC}">
   <dimension ref="A14:U34"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="N14" sqref="N14:U16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
     <row r="14" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A14" s="6" t="s">
+      <c r="A14" s="14" t="s">
         <v>33</v>
       </c>
-      <c r="B14" s="6"/>
-      <c r="C14" s="6"/>
-      <c r="D14" s="6"/>
-      <c r="E14" s="6"/>
-      <c r="F14" s="6"/>
-      <c r="G14" s="6"/>
-      <c r="H14" s="6"/>
-      <c r="I14" s="6"/>
-      <c r="J14" s="6"/>
-      <c r="K14" s="6"/>
-      <c r="N14" s="6" t="s">
+      <c r="B14" s="14"/>
+      <c r="C14" s="14"/>
+      <c r="D14" s="14"/>
+      <c r="E14" s="14"/>
+      <c r="F14" s="14"/>
+      <c r="G14" s="14"/>
+      <c r="H14" s="14"/>
+      <c r="I14" s="14"/>
+      <c r="J14" s="14"/>
+      <c r="K14" s="14"/>
+      <c r="N14" s="14" t="s">
         <v>34</v>
       </c>
-      <c r="O14" s="6"/>
-      <c r="P14" s="6"/>
-      <c r="Q14" s="6"/>
-      <c r="R14" s="6"/>
-      <c r="S14" s="6"/>
-      <c r="T14" s="6"/>
-      <c r="U14" s="6"/>
+      <c r="O14" s="14"/>
+      <c r="P14" s="14"/>
+      <c r="Q14" s="14"/>
+      <c r="R14" s="14"/>
+      <c r="S14" s="14"/>
+      <c r="T14" s="14"/>
+      <c r="U14" s="14"/>
     </row>
     <row r="15" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A15" s="6"/>
-      <c r="B15" s="6"/>
-      <c r="C15" s="6"/>
-      <c r="D15" s="6"/>
-      <c r="E15" s="6"/>
-      <c r="F15" s="6"/>
-      <c r="G15" s="6"/>
-      <c r="H15" s="6"/>
-      <c r="I15" s="6"/>
-      <c r="J15" s="6"/>
-      <c r="K15" s="6"/>
-      <c r="N15" s="6"/>
-      <c r="O15" s="6"/>
-      <c r="P15" s="6"/>
-      <c r="Q15" s="6"/>
-      <c r="R15" s="6"/>
-      <c r="S15" s="6"/>
-      <c r="T15" s="6"/>
-      <c r="U15" s="6"/>
+      <c r="A15" s="14"/>
+      <c r="B15" s="14"/>
+      <c r="C15" s="14"/>
+      <c r="D15" s="14"/>
+      <c r="E15" s="14"/>
+      <c r="F15" s="14"/>
+      <c r="G15" s="14"/>
+      <c r="H15" s="14"/>
+      <c r="I15" s="14"/>
+      <c r="J15" s="14"/>
+      <c r="K15" s="14"/>
+      <c r="N15" s="14"/>
+      <c r="O15" s="14"/>
+      <c r="P15" s="14"/>
+      <c r="Q15" s="14"/>
+      <c r="R15" s="14"/>
+      <c r="S15" s="14"/>
+      <c r="T15" s="14"/>
+      <c r="U15" s="14"/>
     </row>
     <row r="16" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A16" s="6"/>
-      <c r="B16" s="6"/>
-      <c r="C16" s="6"/>
-      <c r="D16" s="6"/>
-      <c r="E16" s="6"/>
-      <c r="F16" s="6"/>
-      <c r="G16" s="6"/>
-      <c r="H16" s="6"/>
-      <c r="I16" s="6"/>
-      <c r="J16" s="6"/>
-      <c r="K16" s="6"/>
-      <c r="N16" s="6"/>
-      <c r="O16" s="6"/>
-      <c r="P16" s="6"/>
-      <c r="Q16" s="6"/>
-      <c r="R16" s="6"/>
-      <c r="S16" s="6"/>
-      <c r="T16" s="6"/>
-      <c r="U16" s="6"/>
+      <c r="A16" s="14"/>
+      <c r="B16" s="14"/>
+      <c r="C16" s="14"/>
+      <c r="D16" s="14"/>
+      <c r="E16" s="14"/>
+      <c r="F16" s="14"/>
+      <c r="G16" s="14"/>
+      <c r="H16" s="14"/>
+      <c r="I16" s="14"/>
+      <c r="J16" s="14"/>
+      <c r="K16" s="14"/>
+      <c r="N16" s="14"/>
+      <c r="O16" s="14"/>
+      <c r="P16" s="14"/>
+      <c r="Q16" s="14"/>
+      <c r="R16" s="14"/>
+      <c r="S16" s="14"/>
+      <c r="T16" s="14"/>
+      <c r="U16" s="14"/>
     </row>
     <row r="30" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A30" t="s">

</xml_diff>